<commit_message>
changes in java files, excel and feature files
</commit_message>
<xml_diff>
--- a/SeleniumCucumberMavenSample/excel-resources/Testdata.xlsx
+++ b/SeleniumCucumberMavenSample/excel-resources/Testdata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11955" windowHeight="4995" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11955" windowHeight="4995" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="data1" sheetId="5" r:id="rId2"/>
     <sheet name="data2" sheetId="6" r:id="rId3"/>
+    <sheet name="data3" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t>Travellers</t>
   </si>
@@ -148,13 +149,89 @@
   </si>
   <si>
     <t>RUN_STATUS</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>EMAIL_ID</t>
+  </si>
+  <si>
+    <t>kaushik.0407@gmail.com</t>
+  </si>
+  <si>
+    <t>kaushik.0407@yahoo.com</t>
+  </si>
+  <si>
+    <t>kaushik.0407@rediffmail.com</t>
+  </si>
+  <si>
+    <t>kaushik.0407@hotmail.com</t>
+  </si>
+  <si>
+    <t>kaushik.0407@apple.com</t>
+  </si>
+  <si>
+    <t>User or Password is not valid</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>User-ID must not be blank</t>
+  </si>
+  <si>
+    <t>Password must not be blank</t>
+  </si>
+  <si>
+    <t>mngr299505</t>
+  </si>
+  <si>
+    <t>nYdAvun</t>
+  </si>
+  <si>
+    <t>mngr299523</t>
+  </si>
+  <si>
+    <t>AhujYtu</t>
+  </si>
+  <si>
+    <t>mngr299525</t>
+  </si>
+  <si>
+    <t>vEvUmAr</t>
+  </si>
+  <si>
+    <t>mngr299524</t>
+  </si>
+  <si>
+    <t>ArEbUmu</t>
+  </si>
+  <si>
+    <t>mngr299515</t>
+  </si>
+  <si>
+    <t>durugEj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +246,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,18 +293,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,8 +619,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="16" spans="1:2">
@@ -578,15 +668,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E6"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="36.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -616,6 +706,12 @@
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
@@ -627,6 +723,12 @@
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
@@ -638,6 +740,12 @@
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
@@ -649,6 +757,12 @@
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
@@ -659,6 +773,12 @@
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -671,18 +791,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -715,6 +835,15 @@
       <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
@@ -726,6 +855,15 @@
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
@@ -737,6 +875,15 @@
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
@@ -748,6 +895,15 @@
       <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
@@ -759,8 +915,148 @@
       <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3:B6" r:id="rId2" display="kaushik.0407@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>